<commit_message>
Prod Diseño Sem 37
</commit_message>
<xml_diff>
--- a/datasets/produccion.xlsx
+++ b/datasets/produccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{58B8D813-9255-4857-99A0-53D4B4D031FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A050E7E5-2CE7-4FF0-9AFE-45884F999345}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{58B8D813-9255-4857-99A0-53D4B4D031FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC4D2E3-680A-47B4-B5AE-FD1FA2C65D34}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{B4B7E62A-ACE4-488F-B31E-63058BE35439}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9940" uniqueCount="3086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10174" uniqueCount="3169">
   <si>
     <t>COD</t>
   </si>
@@ -9294,6 +9294,255 @@
   </si>
   <si>
     <t>6;45542;Entregables</t>
+  </si>
+  <si>
+    <t>1;45544;Entregables</t>
+  </si>
+  <si>
+    <t>pta retrabajo</t>
+  </si>
+  <si>
+    <t>1;45544;Extras</t>
+  </si>
+  <si>
+    <t>VISTA VERDE L-35</t>
+  </si>
+  <si>
+    <t>4 Pergolados</t>
+  </si>
+  <si>
+    <t>2;45544;Extras</t>
+  </si>
+  <si>
+    <t>3;45544;Extras</t>
+  </si>
+  <si>
+    <t>VERONESA C6</t>
+  </si>
+  <si>
+    <t>4;45544;Extras</t>
+  </si>
+  <si>
+    <t>VERONESA (C4-5)</t>
+  </si>
+  <si>
+    <t>5;45544;Extras</t>
+  </si>
+  <si>
+    <t>VERONESA C4</t>
+  </si>
+  <si>
+    <t>6;45544;Extras</t>
+  </si>
+  <si>
+    <t>7;45544;Extras</t>
+  </si>
+  <si>
+    <t>1p cto Maq.</t>
+  </si>
+  <si>
+    <t>8;45544;Extras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HERCOM </t>
+  </si>
+  <si>
+    <t>1O Vistas</t>
+  </si>
+  <si>
+    <t>1;45544;Retrabajos</t>
+  </si>
+  <si>
+    <t>VISTA VERDE L-17</t>
+  </si>
+  <si>
+    <t>2 Pergolados</t>
+  </si>
+  <si>
+    <t>2;45544;Retrabajos</t>
+  </si>
+  <si>
+    <t>VISTA VERDE L-1</t>
+  </si>
+  <si>
+    <t>3;45544;Retrabajos</t>
+  </si>
+  <si>
+    <t>1;45545;Entregables</t>
+  </si>
+  <si>
+    <t>cristina barba</t>
+  </si>
+  <si>
+    <t>librero</t>
+  </si>
+  <si>
+    <t>2;45545;Entregables</t>
+  </si>
+  <si>
+    <t>miguel maldonado</t>
+  </si>
+  <si>
+    <t>lambrin mdb</t>
+  </si>
+  <si>
+    <t>3;45545;Entregables</t>
+  </si>
+  <si>
+    <t>hercom 302</t>
+  </si>
+  <si>
+    <t>4;45545;Entregables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extnsion </t>
+  </si>
+  <si>
+    <t>5;45545;Entregables</t>
+  </si>
+  <si>
+    <t>depto 503 Ta injesa</t>
+  </si>
+  <si>
+    <t>4 pta</t>
+  </si>
+  <si>
+    <t>6;45545;Entregables</t>
+  </si>
+  <si>
+    <t>1;45546;Entregables</t>
+  </si>
+  <si>
+    <t>javier media</t>
+  </si>
+  <si>
+    <t>2;45546;Entregables</t>
+  </si>
+  <si>
+    <t>despacho Gm</t>
+  </si>
+  <si>
+    <t>front desk</t>
+  </si>
+  <si>
+    <t>3;45546;Entregables</t>
+  </si>
+  <si>
+    <t>depto 603 ta injesa</t>
+  </si>
+  <si>
+    <t>4;45546;Entregables</t>
+  </si>
+  <si>
+    <t>5;45546;Entregables</t>
+  </si>
+  <si>
+    <t>2 mdb</t>
+  </si>
+  <si>
+    <t>6;45546;Entregables</t>
+  </si>
+  <si>
+    <t>2 repisas</t>
+  </si>
+  <si>
+    <t>1;45547;Entregables</t>
+  </si>
+  <si>
+    <t>depto 603 TA injesa</t>
+  </si>
+  <si>
+    <t>2;45547;Entregables</t>
+  </si>
+  <si>
+    <t>vista verde l 34</t>
+  </si>
+  <si>
+    <t>pta ppal</t>
+  </si>
+  <si>
+    <t>3;45547;Entregables</t>
+  </si>
+  <si>
+    <t>vista verde l35</t>
+  </si>
+  <si>
+    <t>6 ptas inter</t>
+  </si>
+  <si>
+    <t>4;45547;Entregables</t>
+  </si>
+  <si>
+    <t>pta corrediza</t>
+  </si>
+  <si>
+    <t>5;45547;Entregables</t>
+  </si>
+  <si>
+    <t>veronica eron</t>
+  </si>
+  <si>
+    <t>mueble tv</t>
+  </si>
+  <si>
+    <t>1;45548;Entregables</t>
+  </si>
+  <si>
+    <t>centro capital</t>
+  </si>
+  <si>
+    <t>escritorio en L</t>
+  </si>
+  <si>
+    <t>2;45548;Entregables</t>
+  </si>
+  <si>
+    <t>lambrin mas pta</t>
+  </si>
+  <si>
+    <t>3;45548;Entregables</t>
+  </si>
+  <si>
+    <t>muro divisorio</t>
+  </si>
+  <si>
+    <t>4;45548;Entregables</t>
+  </si>
+  <si>
+    <t>Veronica eron</t>
+  </si>
+  <si>
+    <t>recumbrimiento campana</t>
+  </si>
+  <si>
+    <t>5;45548;Entregables</t>
+  </si>
+  <si>
+    <t>1;45549;Entregables</t>
+  </si>
+  <si>
+    <t>Vista verde l35</t>
+  </si>
+  <si>
+    <t>2;45549;Entregables</t>
+  </si>
+  <si>
+    <t>3;45549;Entregables</t>
+  </si>
+  <si>
+    <t>hercom 301</t>
+  </si>
+  <si>
+    <t>4;45549;Entregables</t>
+  </si>
+  <si>
+    <t>5;45549;Entregables</t>
+  </si>
+  <si>
+    <t>VERONICA ERON</t>
+  </si>
+  <si>
+    <t>1 pta inter</t>
   </si>
 </sst>
 </file>
@@ -9360,13 +9609,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A02BC692-0D78-4DFA-B728-8138C44CDB02}" name="Tabla1" displayName="Tabla1" ref="A1:K1717" totalsRowShown="0">
-  <autoFilter ref="A1:K1717" xr:uid="{A02BC692-0D78-4DFA-B728-8138C44CDB02}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A02BC692-0D78-4DFA-B728-8138C44CDB02}" name="Tabla1" displayName="Tabla1" ref="A1:K1756" totalsRowShown="0">
+  <autoFilter ref="A1:K1756" xr:uid="{A02BC692-0D78-4DFA-B728-8138C44CDB02}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B6ECC9CA-BE29-4C5B-9606-01CFB697A054}" name="COD"/>
     <tableColumn id="2" xr3:uid="{C7D7DD62-79C4-4423-B87E-1408D1237598}" name="CTVV" dataDxfId="2"/>
@@ -9701,10 +9946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEF2190-C283-43C9-B0E2-E2F3DD6D60C6}">
-  <dimension ref="A1:K1717"/>
+  <dimension ref="A1:K1756"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1691" workbookViewId="0">
-      <selection activeCell="I1702" sqref="I1702"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1703" workbookViewId="0">
+      <selection activeCell="J1707" sqref="J1707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -66201,7 +66446,7 @@
       <c r="A1634" t="s">
         <v>2967</v>
       </c>
-      <c r="B1634" s="2" t="s">
+      <c r="B1634" t="s">
         <v>550</v>
       </c>
       <c r="C1634" t="s">
@@ -66216,7 +66461,7 @@
       <c r="F1634">
         <v>1</v>
       </c>
-      <c r="G1634" s="2">
+      <c r="G1634">
         <v>4.5</v>
       </c>
       <c r="H1634" s="1">
@@ -66236,7 +66481,7 @@
       <c r="A1635" t="s">
         <v>2970</v>
       </c>
-      <c r="B1635" s="2" t="s">
+      <c r="B1635" t="s">
         <v>550</v>
       </c>
       <c r="C1635" t="s">
@@ -66251,7 +66496,7 @@
       <c r="F1635">
         <v>1</v>
       </c>
-      <c r="G1635" s="2">
+      <c r="G1635">
         <v>4.5</v>
       </c>
       <c r="H1635" s="1">
@@ -66271,7 +66516,7 @@
       <c r="A1636" t="s">
         <v>2971</v>
       </c>
-      <c r="B1636" s="2" t="s">
+      <c r="B1636" t="s">
         <v>550</v>
       </c>
       <c r="C1636" t="s">
@@ -66286,7 +66531,7 @@
       <c r="F1636">
         <v>1</v>
       </c>
-      <c r="G1636" s="2">
+      <c r="G1636">
         <v>1.7</v>
       </c>
       <c r="H1636" s="1">
@@ -66306,7 +66551,7 @@
       <c r="A1637" t="s">
         <v>2973</v>
       </c>
-      <c r="B1637" s="2" t="s">
+      <c r="B1637" t="s">
         <v>550</v>
       </c>
       <c r="C1637" t="s">
@@ -66321,7 +66566,7 @@
       <c r="F1637">
         <v>1</v>
       </c>
-      <c r="G1637" s="2">
+      <c r="G1637">
         <v>1</v>
       </c>
       <c r="H1637" s="1">
@@ -66341,7 +66586,7 @@
       <c r="A1638" t="s">
         <v>2976</v>
       </c>
-      <c r="B1638" s="2" t="s">
+      <c r="B1638" t="s">
         <v>550</v>
       </c>
       <c r="C1638" t="s">
@@ -66356,7 +66601,7 @@
       <c r="F1638">
         <v>1</v>
       </c>
-      <c r="G1638" s="2">
+      <c r="G1638">
         <v>2</v>
       </c>
       <c r="H1638" s="1">
@@ -66376,7 +66621,7 @@
       <c r="A1639" t="s">
         <v>2978</v>
       </c>
-      <c r="B1639" s="2" t="s">
+      <c r="B1639" t="s">
         <v>965</v>
       </c>
       <c r="C1639" t="s">
@@ -66391,7 +66636,7 @@
       <c r="F1639">
         <v>1</v>
       </c>
-      <c r="G1639" s="2">
+      <c r="G1639">
         <v>2</v>
       </c>
       <c r="H1639" s="1">
@@ -66411,7 +66656,7 @@
       <c r="A1640" t="s">
         <v>2980</v>
       </c>
-      <c r="B1640" s="2" t="s">
+      <c r="B1640" t="s">
         <v>550</v>
       </c>
       <c r="C1640" t="s">
@@ -66426,7 +66671,7 @@
       <c r="F1640">
         <v>2</v>
       </c>
-      <c r="G1640" s="2">
+      <c r="G1640">
         <v>1</v>
       </c>
       <c r="H1640" s="1">
@@ -66446,7 +66691,7 @@
       <c r="A1641" t="s">
         <v>2982</v>
       </c>
-      <c r="B1641" s="2" t="s">
+      <c r="B1641" t="s">
         <v>550</v>
       </c>
       <c r="C1641" t="s">
@@ -66461,7 +66706,7 @@
       <c r="F1641">
         <v>1</v>
       </c>
-      <c r="G1641" s="2">
+      <c r="G1641">
         <v>1</v>
       </c>
       <c r="H1641" s="1">
@@ -66481,7 +66726,7 @@
       <c r="A1642" t="s">
         <v>2983</v>
       </c>
-      <c r="B1642" s="2" t="s">
+      <c r="B1642" t="s">
         <v>1507</v>
       </c>
       <c r="C1642" t="s">
@@ -66496,7 +66741,7 @@
       <c r="F1642">
         <v>1</v>
       </c>
-      <c r="G1642" s="2">
+      <c r="G1642">
         <v>0.5</v>
       </c>
       <c r="H1642" s="1">
@@ -66516,7 +66761,7 @@
       <c r="A1643" t="s">
         <v>2985</v>
       </c>
-      <c r="B1643" s="2" t="s">
+      <c r="B1643" t="s">
         <v>1507</v>
       </c>
       <c r="C1643" t="s">
@@ -66531,7 +66776,7 @@
       <c r="F1643">
         <v>1</v>
       </c>
-      <c r="G1643" s="2">
+      <c r="G1643">
         <v>0.5</v>
       </c>
       <c r="H1643" s="1">
@@ -66551,7 +66796,7 @@
       <c r="A1644" t="s">
         <v>2986</v>
       </c>
-      <c r="B1644" s="2" t="s">
+      <c r="B1644" t="s">
         <v>550</v>
       </c>
       <c r="C1644" t="s">
@@ -66566,7 +66811,7 @@
       <c r="F1644">
         <v>1</v>
       </c>
-      <c r="G1644" s="2">
+      <c r="G1644">
         <v>1</v>
       </c>
       <c r="H1644" s="1">
@@ -66586,7 +66831,7 @@
       <c r="A1645" t="s">
         <v>2987</v>
       </c>
-      <c r="B1645" s="2" t="s">
+      <c r="B1645" t="s">
         <v>550</v>
       </c>
       <c r="C1645" t="s">
@@ -66601,7 +66846,7 @@
       <c r="F1645">
         <v>1</v>
       </c>
-      <c r="G1645" s="2">
+      <c r="G1645">
         <v>2</v>
       </c>
       <c r="H1645" s="1">
@@ -66621,7 +66866,7 @@
       <c r="A1646" t="s">
         <v>2988</v>
       </c>
-      <c r="B1646" s="2" t="s">
+      <c r="B1646" t="s">
         <v>550</v>
       </c>
       <c r="C1646" t="s">
@@ -66636,7 +66881,7 @@
       <c r="F1646">
         <v>1</v>
       </c>
-      <c r="G1646" s="2">
+      <c r="G1646">
         <v>1</v>
       </c>
       <c r="H1646" s="1">
@@ -66656,7 +66901,7 @@
       <c r="A1647" t="s">
         <v>2990</v>
       </c>
-      <c r="B1647" s="2" t="s">
+      <c r="B1647" t="s">
         <v>550</v>
       </c>
       <c r="C1647" t="s">
@@ -66671,7 +66916,7 @@
       <c r="F1647">
         <v>1</v>
       </c>
-      <c r="G1647" s="2">
+      <c r="G1647">
         <v>0.6</v>
       </c>
       <c r="H1647" s="1">
@@ -66691,7 +66936,7 @@
       <c r="A1648" t="s">
         <v>2992</v>
       </c>
-      <c r="B1648" s="2" t="s">
+      <c r="B1648" t="s">
         <v>550</v>
       </c>
       <c r="C1648" t="s">
@@ -66703,7 +66948,7 @@
       <c r="F1648">
         <v>1</v>
       </c>
-      <c r="G1648" s="2">
+      <c r="G1648">
         <v>0</v>
       </c>
       <c r="H1648" s="1">
@@ -66723,7 +66968,7 @@
       <c r="A1649" t="s">
         <v>2995</v>
       </c>
-      <c r="B1649" s="2" t="s">
+      <c r="B1649" t="s">
         <v>550</v>
       </c>
       <c r="C1649" t="s">
@@ -66738,7 +66983,7 @@
       <c r="F1649">
         <v>0</v>
       </c>
-      <c r="G1649" s="2">
+      <c r="G1649">
         <v>0</v>
       </c>
       <c r="H1649" s="1">
@@ -66758,7 +67003,7 @@
       <c r="A1650" t="s">
         <v>2997</v>
       </c>
-      <c r="B1650" s="2" t="s">
+      <c r="B1650" t="s">
         <v>550</v>
       </c>
       <c r="C1650" t="s">
@@ -66773,7 +67018,7 @@
       <c r="F1650">
         <v>1</v>
       </c>
-      <c r="G1650" s="2">
+      <c r="G1650">
         <v>1.5</v>
       </c>
       <c r="H1650" s="1">
@@ -66793,7 +67038,7 @@
       <c r="A1651" t="s">
         <v>2998</v>
       </c>
-      <c r="B1651" s="2" t="s">
+      <c r="B1651" t="s">
         <v>550</v>
       </c>
       <c r="C1651" t="s">
@@ -66808,7 +67053,7 @@
       <c r="F1651">
         <v>1</v>
       </c>
-      <c r="G1651" s="2">
+      <c r="G1651">
         <v>1.8</v>
       </c>
       <c r="H1651" s="1">
@@ -66828,7 +67073,7 @@
       <c r="A1652" t="s">
         <v>2999</v>
       </c>
-      <c r="B1652" s="2" t="s">
+      <c r="B1652" t="s">
         <v>550</v>
       </c>
       <c r="C1652" t="s">
@@ -66843,7 +67088,7 @@
       <c r="F1652">
         <v>0</v>
       </c>
-      <c r="G1652" s="2">
+      <c r="G1652">
         <v>0</v>
       </c>
       <c r="H1652" s="1">
@@ -66863,7 +67108,7 @@
       <c r="A1653" t="s">
         <v>3000</v>
       </c>
-      <c r="B1653" s="2" t="s">
+      <c r="B1653" t="s">
         <v>550</v>
       </c>
       <c r="C1653" t="s">
@@ -66878,7 +67123,7 @@
       <c r="F1653">
         <v>1</v>
       </c>
-      <c r="G1653" s="2">
+      <c r="G1653">
         <v>1.8</v>
       </c>
       <c r="H1653" s="1">
@@ -66898,7 +67143,7 @@
       <c r="A1654" t="s">
         <v>3002</v>
       </c>
-      <c r="B1654" s="2" t="s">
+      <c r="B1654" t="s">
         <v>550</v>
       </c>
       <c r="C1654" t="s">
@@ -66910,7 +67155,7 @@
       <c r="F1654">
         <v>1</v>
       </c>
-      <c r="G1654" s="2">
+      <c r="G1654">
         <v>0</v>
       </c>
       <c r="H1654" s="1">
@@ -66930,7 +67175,7 @@
       <c r="A1655" t="s">
         <v>3005</v>
       </c>
-      <c r="B1655" s="2" t="s">
+      <c r="B1655" t="s">
         <v>550</v>
       </c>
       <c r="C1655" t="s">
@@ -66945,7 +67190,7 @@
       <c r="F1655">
         <v>1</v>
       </c>
-      <c r="G1655" s="2">
+      <c r="G1655">
         <v>2</v>
       </c>
       <c r="H1655" s="1">
@@ -66965,7 +67210,7 @@
       <c r="A1656" t="s">
         <v>3007</v>
       </c>
-      <c r="B1656" s="2" t="s">
+      <c r="B1656" t="s">
         <v>550</v>
       </c>
       <c r="C1656" t="s">
@@ -66980,7 +67225,7 @@
       <c r="F1656">
         <v>0</v>
       </c>
-      <c r="G1656" s="2">
+      <c r="G1656">
         <v>0</v>
       </c>
       <c r="H1656" s="1">
@@ -67000,7 +67245,7 @@
       <c r="A1657" t="s">
         <v>3008</v>
       </c>
-      <c r="B1657" s="2" t="s">
+      <c r="B1657" t="s">
         <v>550</v>
       </c>
       <c r="C1657" t="s">
@@ -67015,7 +67260,7 @@
       <c r="F1657">
         <v>1</v>
       </c>
-      <c r="G1657" s="2">
+      <c r="G1657">
         <v>7.5</v>
       </c>
       <c r="H1657" s="1">
@@ -67035,7 +67280,7 @@
       <c r="A1658" t="s">
         <v>3009</v>
       </c>
-      <c r="B1658" s="2" t="s">
+      <c r="B1658" t="s">
         <v>550</v>
       </c>
       <c r="C1658" t="s">
@@ -67050,7 +67295,7 @@
       <c r="F1658">
         <v>1</v>
       </c>
-      <c r="G1658" s="2">
+      <c r="G1658">
         <v>0.7</v>
       </c>
       <c r="H1658" s="1">
@@ -67070,7 +67315,7 @@
       <c r="A1659" t="s">
         <v>3010</v>
       </c>
-      <c r="B1659" s="2" t="s">
+      <c r="B1659" t="s">
         <v>550</v>
       </c>
       <c r="C1659" t="s">
@@ -67085,7 +67330,7 @@
       <c r="F1659">
         <v>0</v>
       </c>
-      <c r="G1659" s="2">
+      <c r="G1659">
         <v>0</v>
       </c>
       <c r="H1659" s="1">
@@ -67105,7 +67350,7 @@
       <c r="A1660" t="s">
         <v>3012</v>
       </c>
-      <c r="B1660" s="2" t="s">
+      <c r="B1660" t="s">
         <v>550</v>
       </c>
       <c r="C1660" t="s">
@@ -67117,7 +67362,7 @@
       <c r="F1660">
         <v>1</v>
       </c>
-      <c r="G1660" s="2">
+      <c r="G1660">
         <v>0</v>
       </c>
       <c r="H1660" s="1">
@@ -67137,7 +67382,7 @@
       <c r="A1661" t="s">
         <v>3014</v>
       </c>
-      <c r="B1661" s="2" t="s">
+      <c r="B1661" t="s">
         <v>550</v>
       </c>
       <c r="C1661" t="s">
@@ -67152,7 +67397,7 @@
       <c r="F1661">
         <v>1</v>
       </c>
-      <c r="G1661" s="2">
+      <c r="G1661">
         <v>9.1</v>
       </c>
       <c r="H1661" s="1">
@@ -67172,7 +67417,7 @@
       <c r="A1662" t="s">
         <v>3017</v>
       </c>
-      <c r="B1662" s="2" t="s">
+      <c r="B1662" t="s">
         <v>550</v>
       </c>
       <c r="C1662" t="s">
@@ -67187,7 +67432,7 @@
       <c r="F1662">
         <v>1</v>
       </c>
-      <c r="G1662" s="2">
+      <c r="G1662">
         <v>3</v>
       </c>
       <c r="H1662" s="1">
@@ -67207,7 +67452,7 @@
       <c r="A1663" t="s">
         <v>3019</v>
       </c>
-      <c r="B1663" s="2" t="s">
+      <c r="B1663" t="s">
         <v>1202</v>
       </c>
       <c r="C1663" t="s">
@@ -67222,7 +67467,7 @@
       <c r="F1663">
         <v>1</v>
       </c>
-      <c r="G1663" s="2">
+      <c r="G1663">
         <v>1.4</v>
       </c>
       <c r="H1663" s="1">
@@ -67242,7 +67487,7 @@
       <c r="A1664" t="s">
         <v>3020</v>
       </c>
-      <c r="B1664" s="2" t="s">
+      <c r="B1664" t="s">
         <v>550</v>
       </c>
       <c r="C1664" t="s">
@@ -67254,7 +67499,7 @@
       <c r="F1664">
         <v>1</v>
       </c>
-      <c r="G1664" s="2">
+      <c r="G1664">
         <v>0</v>
       </c>
       <c r="H1664" s="1">
@@ -67274,7 +67519,7 @@
       <c r="A1665" t="s">
         <v>3022</v>
       </c>
-      <c r="B1665" s="2" t="s">
+      <c r="B1665" t="s">
         <v>550</v>
       </c>
       <c r="C1665" t="s">
@@ -67286,7 +67531,7 @@
       <c r="F1665">
         <v>1</v>
       </c>
-      <c r="G1665" s="2">
+      <c r="G1665">
         <v>0</v>
       </c>
       <c r="H1665" s="1">
@@ -67306,7 +67551,7 @@
       <c r="A1666" t="s">
         <v>3025</v>
       </c>
-      <c r="B1666" s="2" t="s">
+      <c r="B1666" t="s">
         <v>550</v>
       </c>
       <c r="C1666" t="s">
@@ -67321,7 +67566,7 @@
       <c r="F1666">
         <v>1</v>
       </c>
-      <c r="G1666" s="2">
+      <c r="G1666">
         <v>1.2</v>
       </c>
       <c r="H1666" s="1">
@@ -67341,7 +67586,7 @@
       <c r="A1667" t="s">
         <v>3028</v>
       </c>
-      <c r="B1667" s="2" t="s">
+      <c r="B1667" t="s">
         <v>550</v>
       </c>
       <c r="C1667" t="s">
@@ -67356,7 +67601,7 @@
       <c r="F1667">
         <v>0</v>
       </c>
-      <c r="G1667" s="2">
+      <c r="G1667">
         <v>0</v>
       </c>
       <c r="H1667" s="1">
@@ -67376,7 +67621,7 @@
       <c r="A1668" t="s">
         <v>3030</v>
       </c>
-      <c r="B1668" s="2" t="s">
+      <c r="B1668" t="s">
         <v>550</v>
       </c>
       <c r="C1668" t="s">
@@ -67391,7 +67636,7 @@
       <c r="F1668">
         <v>1</v>
       </c>
-      <c r="G1668" s="2">
+      <c r="G1668">
         <v>1.9</v>
       </c>
       <c r="H1668" s="1">
@@ -67411,7 +67656,7 @@
       <c r="A1669" t="s">
         <v>3032</v>
       </c>
-      <c r="B1669" s="2" t="s">
+      <c r="B1669" t="s">
         <v>550</v>
       </c>
       <c r="C1669" t="s">
@@ -67426,7 +67671,7 @@
       <c r="F1669">
         <v>1</v>
       </c>
-      <c r="G1669" s="2">
+      <c r="G1669">
         <v>0.5</v>
       </c>
       <c r="H1669" s="1">
@@ -67446,7 +67691,7 @@
       <c r="A1670" t="s">
         <v>3033</v>
       </c>
-      <c r="B1670" s="2" t="s">
+      <c r="B1670" t="s">
         <v>550</v>
       </c>
       <c r="C1670" t="s">
@@ -67461,7 +67706,7 @@
       <c r="F1670">
         <v>0</v>
       </c>
-      <c r="G1670" s="2">
+      <c r="G1670">
         <v>0</v>
       </c>
       <c r="H1670" s="1">
@@ -67481,7 +67726,7 @@
       <c r="A1671" t="s">
         <v>3036</v>
       </c>
-      <c r="B1671" s="2" t="s">
+      <c r="B1671" t="s">
         <v>550</v>
       </c>
       <c r="C1671" t="s">
@@ -67496,7 +67741,7 @@
       <c r="F1671">
         <v>1</v>
       </c>
-      <c r="G1671" s="2">
+      <c r="G1671">
         <v>3.2</v>
       </c>
       <c r="H1671" s="1">
@@ -67516,7 +67761,7 @@
       <c r="A1672" t="s">
         <v>3037</v>
       </c>
-      <c r="B1672" s="2" t="s">
+      <c r="B1672" t="s">
         <v>550</v>
       </c>
       <c r="C1672" t="s">
@@ -67531,7 +67776,7 @@
       <c r="F1672">
         <v>1</v>
       </c>
-      <c r="G1672" s="2">
+      <c r="G1672">
         <v>3.2</v>
       </c>
       <c r="H1672" s="1">
@@ -67551,7 +67796,7 @@
       <c r="A1673" t="s">
         <v>3038</v>
       </c>
-      <c r="B1673" s="2" t="s">
+      <c r="B1673" t="s">
         <v>550</v>
       </c>
       <c r="C1673" t="s">
@@ -67566,7 +67811,7 @@
       <c r="F1673">
         <v>1</v>
       </c>
-      <c r="G1673" s="2">
+      <c r="G1673">
         <v>4.7</v>
       </c>
       <c r="H1673" s="1">
@@ -67586,7 +67831,7 @@
       <c r="A1674" t="s">
         <v>3040</v>
       </c>
-      <c r="B1674" s="2" t="s">
+      <c r="B1674" t="s">
         <v>550</v>
       </c>
       <c r="C1674" t="s">
@@ -67601,7 +67846,7 @@
       <c r="F1674">
         <v>1</v>
       </c>
-      <c r="G1674" s="2">
+      <c r="G1674">
         <v>1.1000000000000001</v>
       </c>
       <c r="H1674" s="1">
@@ -67621,7 +67866,7 @@
       <c r="A1675" t="s">
         <v>3042</v>
       </c>
-      <c r="B1675" s="2" t="s">
+      <c r="B1675" t="s">
         <v>550</v>
       </c>
       <c r="C1675" t="s">
@@ -67636,7 +67881,7 @@
       <c r="F1675">
         <v>1</v>
       </c>
-      <c r="G1675" s="2">
+      <c r="G1675">
         <v>1.5</v>
       </c>
       <c r="H1675" s="1">
@@ -67656,7 +67901,7 @@
       <c r="A1676" t="s">
         <v>3044</v>
       </c>
-      <c r="B1676" s="2" t="s">
+      <c r="B1676" t="s">
         <v>550</v>
       </c>
       <c r="C1676" t="s">
@@ -67671,7 +67916,7 @@
       <c r="F1676">
         <v>1</v>
       </c>
-      <c r="G1676" s="2">
+      <c r="G1676">
         <v>4.5</v>
       </c>
       <c r="H1676" s="1">
@@ -67691,7 +67936,7 @@
       <c r="A1677" t="s">
         <v>3045</v>
       </c>
-      <c r="B1677" s="2" t="s">
+      <c r="B1677" t="s">
         <v>550</v>
       </c>
       <c r="C1677" t="s">
@@ -67706,7 +67951,7 @@
       <c r="F1677">
         <v>1</v>
       </c>
-      <c r="G1677" s="2">
+      <c r="G1677">
         <v>4.5</v>
       </c>
       <c r="H1677" s="1">
@@ -67726,7 +67971,7 @@
       <c r="A1678" t="s">
         <v>3046</v>
       </c>
-      <c r="B1678" s="2" t="s">
+      <c r="B1678" t="s">
         <v>550</v>
       </c>
       <c r="C1678" t="s">
@@ -67741,7 +67986,7 @@
       <c r="F1678">
         <v>1</v>
       </c>
-      <c r="G1678" s="2">
+      <c r="G1678">
         <v>1.7</v>
       </c>
       <c r="H1678" s="1">
@@ -67761,7 +68006,7 @@
       <c r="A1679" t="s">
         <v>3047</v>
       </c>
-      <c r="B1679" s="2" t="s">
+      <c r="B1679" t="s">
         <v>550</v>
       </c>
       <c r="C1679" t="s">
@@ -67776,7 +68021,7 @@
       <c r="F1679">
         <v>1</v>
       </c>
-      <c r="G1679" s="2">
+      <c r="G1679">
         <v>1</v>
       </c>
       <c r="H1679" s="1">
@@ -67796,7 +68041,7 @@
       <c r="A1680" t="s">
         <v>3048</v>
       </c>
-      <c r="B1680" s="2" t="s">
+      <c r="B1680" t="s">
         <v>550</v>
       </c>
       <c r="C1680" t="s">
@@ -67811,7 +68056,7 @@
       <c r="F1680">
         <v>1</v>
       </c>
-      <c r="G1680" s="2">
+      <c r="G1680">
         <v>2</v>
       </c>
       <c r="H1680" s="1">
@@ -67831,7 +68076,7 @@
       <c r="A1681" t="s">
         <v>3049</v>
       </c>
-      <c r="B1681" s="2" t="s">
+      <c r="B1681" t="s">
         <v>965</v>
       </c>
       <c r="C1681" t="s">
@@ -67846,7 +68091,7 @@
       <c r="F1681">
         <v>1</v>
       </c>
-      <c r="G1681" s="2">
+      <c r="G1681">
         <v>2</v>
       </c>
       <c r="H1681" s="1">
@@ -67866,7 +68111,7 @@
       <c r="A1682" t="s">
         <v>3050</v>
       </c>
-      <c r="B1682" s="2" t="s">
+      <c r="B1682" t="s">
         <v>550</v>
       </c>
       <c r="C1682" t="s">
@@ -67881,7 +68126,7 @@
       <c r="F1682">
         <v>2</v>
       </c>
-      <c r="G1682" s="2">
+      <c r="G1682">
         <v>1</v>
       </c>
       <c r="H1682" s="1">
@@ -67901,7 +68146,7 @@
       <c r="A1683" t="s">
         <v>3051</v>
       </c>
-      <c r="B1683" s="2" t="s">
+      <c r="B1683" t="s">
         <v>550</v>
       </c>
       <c r="C1683" t="s">
@@ -67916,7 +68161,7 @@
       <c r="F1683">
         <v>1</v>
       </c>
-      <c r="G1683" s="2">
+      <c r="G1683">
         <v>1</v>
       </c>
       <c r="H1683" s="1">
@@ -67936,7 +68181,7 @@
       <c r="A1684" t="s">
         <v>3052</v>
       </c>
-      <c r="B1684" s="2" t="s">
+      <c r="B1684" t="s">
         <v>1507</v>
       </c>
       <c r="C1684" t="s">
@@ -67951,7 +68196,7 @@
       <c r="F1684">
         <v>1</v>
       </c>
-      <c r="G1684" s="2">
+      <c r="G1684">
         <v>0.5</v>
       </c>
       <c r="H1684" s="1">
@@ -67971,7 +68216,7 @@
       <c r="A1685" t="s">
         <v>3053</v>
       </c>
-      <c r="B1685" s="2" t="s">
+      <c r="B1685" t="s">
         <v>1507</v>
       </c>
       <c r="C1685" t="s">
@@ -67986,7 +68231,7 @@
       <c r="F1685">
         <v>1</v>
       </c>
-      <c r="G1685" s="2">
+      <c r="G1685">
         <v>0.5</v>
       </c>
       <c r="H1685" s="1">
@@ -68006,7 +68251,7 @@
       <c r="A1686" t="s">
         <v>3054</v>
       </c>
-      <c r="B1686" s="2" t="s">
+      <c r="B1686" t="s">
         <v>550</v>
       </c>
       <c r="C1686" t="s">
@@ -68021,7 +68266,7 @@
       <c r="F1686">
         <v>1</v>
       </c>
-      <c r="G1686" s="2">
+      <c r="G1686">
         <v>1</v>
       </c>
       <c r="H1686" s="1">
@@ -68041,7 +68286,7 @@
       <c r="A1687" t="s">
         <v>3055</v>
       </c>
-      <c r="B1687" s="2" t="s">
+      <c r="B1687" t="s">
         <v>550</v>
       </c>
       <c r="C1687" t="s">
@@ -68056,7 +68301,7 @@
       <c r="F1687">
         <v>1</v>
       </c>
-      <c r="G1687" s="2">
+      <c r="G1687">
         <v>2</v>
       </c>
       <c r="H1687" s="1">
@@ -68076,7 +68321,7 @@
       <c r="A1688" t="s">
         <v>3056</v>
       </c>
-      <c r="B1688" s="2" t="s">
+      <c r="B1688" t="s">
         <v>550</v>
       </c>
       <c r="C1688" t="s">
@@ -68091,7 +68336,7 @@
       <c r="F1688">
         <v>1</v>
       </c>
-      <c r="G1688" s="2">
+      <c r="G1688">
         <v>1</v>
       </c>
       <c r="H1688" s="1">
@@ -68111,7 +68356,7 @@
       <c r="A1689" t="s">
         <v>3057</v>
       </c>
-      <c r="B1689" s="2" t="s">
+      <c r="B1689" t="s">
         <v>550</v>
       </c>
       <c r="C1689" t="s">
@@ -68126,7 +68371,7 @@
       <c r="F1689">
         <v>1</v>
       </c>
-      <c r="G1689" s="2">
+      <c r="G1689">
         <v>0.6</v>
       </c>
       <c r="H1689" s="1">
@@ -68146,7 +68391,7 @@
       <c r="A1690" t="s">
         <v>3058</v>
       </c>
-      <c r="B1690" s="2" t="s">
+      <c r="B1690" t="s">
         <v>550</v>
       </c>
       <c r="C1690" t="s">
@@ -68158,7 +68403,7 @@
       <c r="F1690">
         <v>1</v>
       </c>
-      <c r="G1690" s="2">
+      <c r="G1690">
         <v>0</v>
       </c>
       <c r="H1690" s="1">
@@ -68178,7 +68423,7 @@
       <c r="A1691" t="s">
         <v>3059</v>
       </c>
-      <c r="B1691" s="2" t="s">
+      <c r="B1691" t="s">
         <v>550</v>
       </c>
       <c r="C1691" t="s">
@@ -68190,7 +68435,7 @@
       <c r="E1691">
         <v>2.7</v>
       </c>
-      <c r="G1691" s="2">
+      <c r="G1691">
         <v>0</v>
       </c>
       <c r="H1691" s="1">
@@ -68210,7 +68455,7 @@
       <c r="A1692" t="s">
         <v>3060</v>
       </c>
-      <c r="B1692" s="2" t="s">
+      <c r="B1692" t="s">
         <v>550</v>
       </c>
       <c r="C1692" t="s">
@@ -68225,7 +68470,7 @@
       <c r="F1692">
         <v>1</v>
       </c>
-      <c r="G1692" s="2">
+      <c r="G1692">
         <v>1.5</v>
       </c>
       <c r="H1692" s="1">
@@ -68245,7 +68490,7 @@
       <c r="A1693" t="s">
         <v>3061</v>
       </c>
-      <c r="B1693" s="2" t="s">
+      <c r="B1693" t="s">
         <v>550</v>
       </c>
       <c r="C1693" t="s">
@@ -68260,7 +68505,7 @@
       <c r="F1693">
         <v>1</v>
       </c>
-      <c r="G1693" s="2">
+      <c r="G1693">
         <v>1.8</v>
       </c>
       <c r="H1693" s="1">
@@ -68280,7 +68525,7 @@
       <c r="A1694" t="s">
         <v>3062</v>
       </c>
-      <c r="B1694" s="2" t="s">
+      <c r="B1694" t="s">
         <v>550</v>
       </c>
       <c r="C1694" t="s">
@@ -68295,7 +68540,7 @@
       <c r="F1694">
         <v>0</v>
       </c>
-      <c r="G1694" s="2">
+      <c r="G1694">
         <v>0</v>
       </c>
       <c r="H1694" s="1">
@@ -68315,7 +68560,7 @@
       <c r="A1695" t="s">
         <v>3063</v>
       </c>
-      <c r="B1695" s="2" t="s">
+      <c r="B1695" t="s">
         <v>550</v>
       </c>
       <c r="C1695" t="s">
@@ -68330,7 +68575,7 @@
       <c r="F1695">
         <v>1</v>
       </c>
-      <c r="G1695" s="2">
+      <c r="G1695">
         <v>1.8</v>
       </c>
       <c r="H1695" s="1">
@@ -68350,7 +68595,7 @@
       <c r="A1696" t="s">
         <v>3064</v>
       </c>
-      <c r="B1696" s="2" t="s">
+      <c r="B1696" t="s">
         <v>550</v>
       </c>
       <c r="C1696" t="s">
@@ -68365,7 +68610,7 @@
       <c r="F1696">
         <v>1</v>
       </c>
-      <c r="G1696" s="2">
+      <c r="G1696">
         <v>1</v>
       </c>
       <c r="H1696" s="1">
@@ -68385,7 +68630,7 @@
       <c r="A1697" t="s">
         <v>3065</v>
       </c>
-      <c r="B1697" s="2" t="s">
+      <c r="B1697" t="s">
         <v>550</v>
       </c>
       <c r="C1697" t="s">
@@ -68400,7 +68645,7 @@
       <c r="F1697">
         <v>1</v>
       </c>
-      <c r="G1697" s="2">
+      <c r="G1697">
         <v>2</v>
       </c>
       <c r="H1697" s="1">
@@ -68420,7 +68665,7 @@
       <c r="A1698" t="s">
         <v>3066</v>
       </c>
-      <c r="B1698" s="2" t="s">
+      <c r="B1698" t="s">
         <v>550</v>
       </c>
       <c r="C1698" t="s">
@@ -68435,7 +68680,7 @@
       <c r="F1698">
         <v>0</v>
       </c>
-      <c r="G1698" s="2">
+      <c r="G1698">
         <v>0</v>
       </c>
       <c r="H1698" s="1">
@@ -68455,7 +68700,7 @@
       <c r="A1699" t="s">
         <v>3067</v>
       </c>
-      <c r="B1699" s="2" t="s">
+      <c r="B1699" t="s">
         <v>550</v>
       </c>
       <c r="C1699" t="s">
@@ -68470,7 +68715,7 @@
       <c r="F1699">
         <v>1</v>
       </c>
-      <c r="G1699" s="2">
+      <c r="G1699">
         <v>7.5</v>
       </c>
       <c r="H1699" s="1">
@@ -68490,7 +68735,7 @@
       <c r="A1700" t="s">
         <v>3068</v>
       </c>
-      <c r="B1700" s="2" t="s">
+      <c r="B1700" t="s">
         <v>550</v>
       </c>
       <c r="C1700" t="s">
@@ -68505,7 +68750,7 @@
       <c r="F1700">
         <v>1</v>
       </c>
-      <c r="G1700" s="2">
+      <c r="G1700">
         <v>0.7</v>
       </c>
       <c r="H1700" s="1">
@@ -68525,7 +68770,7 @@
       <c r="A1701" t="s">
         <v>3069</v>
       </c>
-      <c r="B1701" s="2" t="s">
+      <c r="B1701" t="s">
         <v>550</v>
       </c>
       <c r="C1701" t="s">
@@ -68540,7 +68785,7 @@
       <c r="F1701">
         <v>0</v>
       </c>
-      <c r="G1701" s="2">
+      <c r="G1701">
         <v>0</v>
       </c>
       <c r="H1701" s="1">
@@ -68560,7 +68805,7 @@
       <c r="A1702" t="s">
         <v>3070</v>
       </c>
-      <c r="B1702" s="2" t="s">
+      <c r="B1702" t="s">
         <v>550</v>
       </c>
       <c r="C1702" t="s">
@@ -68572,7 +68817,7 @@
       <c r="F1702">
         <v>1</v>
       </c>
-      <c r="G1702" s="2">
+      <c r="G1702">
         <v>0</v>
       </c>
       <c r="H1702" s="1">
@@ -68592,7 +68837,7 @@
       <c r="A1703" t="s">
         <v>3071</v>
       </c>
-      <c r="B1703" s="2" t="s">
+      <c r="B1703" t="s">
         <v>550</v>
       </c>
       <c r="C1703" t="s">
@@ -68607,7 +68852,7 @@
       <c r="F1703">
         <v>1</v>
       </c>
-      <c r="G1703" s="2">
+      <c r="G1703">
         <v>9.1</v>
       </c>
       <c r="H1703" s="1">
@@ -68627,7 +68872,7 @@
       <c r="A1704" t="s">
         <v>3072</v>
       </c>
-      <c r="B1704" s="2" t="s">
+      <c r="B1704" t="s">
         <v>550</v>
       </c>
       <c r="C1704" t="s">
@@ -68642,7 +68887,7 @@
       <c r="F1704">
         <v>1</v>
       </c>
-      <c r="G1704" s="2">
+      <c r="G1704">
         <v>3</v>
       </c>
       <c r="H1704" s="1">
@@ -68662,7 +68907,7 @@
       <c r="A1705" t="s">
         <v>3073</v>
       </c>
-      <c r="B1705" s="2" t="s">
+      <c r="B1705" t="s">
         <v>1202</v>
       </c>
       <c r="C1705" t="s">
@@ -68677,7 +68922,7 @@
       <c r="F1705">
         <v>1</v>
       </c>
-      <c r="G1705" s="2">
+      <c r="G1705">
         <v>1.4</v>
       </c>
       <c r="H1705" s="1">
@@ -68697,7 +68942,7 @@
       <c r="A1706" t="s">
         <v>3074</v>
       </c>
-      <c r="B1706" s="2" t="s">
+      <c r="B1706" t="s">
         <v>550</v>
       </c>
       <c r="C1706" t="s">
@@ -68709,7 +68954,7 @@
       <c r="F1706">
         <v>1</v>
       </c>
-      <c r="G1706" s="2">
+      <c r="G1706">
         <v>0</v>
       </c>
       <c r="H1706" s="1">
@@ -68729,7 +68974,7 @@
       <c r="A1707" t="s">
         <v>3075</v>
       </c>
-      <c r="B1707" s="2" t="s">
+      <c r="B1707" t="s">
         <v>550</v>
       </c>
       <c r="C1707" t="s">
@@ -68741,7 +68986,7 @@
       <c r="F1707">
         <v>1</v>
       </c>
-      <c r="G1707" s="2">
+      <c r="G1707">
         <v>0</v>
       </c>
       <c r="H1707" s="1">
@@ -68761,7 +69006,7 @@
       <c r="A1708" t="s">
         <v>3076</v>
       </c>
-      <c r="B1708" s="2" t="s">
+      <c r="B1708" t="s">
         <v>550</v>
       </c>
       <c r="C1708" t="s">
@@ -68776,7 +69021,7 @@
       <c r="F1708">
         <v>1</v>
       </c>
-      <c r="G1708" s="2">
+      <c r="G1708">
         <v>1.2</v>
       </c>
       <c r="H1708" s="1">
@@ -68796,7 +69041,7 @@
       <c r="A1709" t="s">
         <v>3077</v>
       </c>
-      <c r="B1709" s="2" t="s">
+      <c r="B1709" t="s">
         <v>550</v>
       </c>
       <c r="C1709" t="s">
@@ -68811,7 +69056,7 @@
       <c r="F1709">
         <v>0</v>
       </c>
-      <c r="G1709" s="2">
+      <c r="G1709">
         <v>0</v>
       </c>
       <c r="H1709" s="1">
@@ -68831,7 +69076,7 @@
       <c r="A1710" t="s">
         <v>3078</v>
       </c>
-      <c r="B1710" s="2" t="s">
+      <c r="B1710" t="s">
         <v>550</v>
       </c>
       <c r="C1710" t="s">
@@ -68846,7 +69091,7 @@
       <c r="F1710">
         <v>1</v>
       </c>
-      <c r="G1710" s="2">
+      <c r="G1710">
         <v>1.9</v>
       </c>
       <c r="H1710" s="1">
@@ -68866,7 +69111,7 @@
       <c r="A1711" t="s">
         <v>3079</v>
       </c>
-      <c r="B1711" s="2" t="s">
+      <c r="B1711" t="s">
         <v>550</v>
       </c>
       <c r="C1711" t="s">
@@ -68881,7 +69126,7 @@
       <c r="F1711">
         <v>1</v>
       </c>
-      <c r="G1711" s="2">
+      <c r="G1711">
         <v>0.5</v>
       </c>
       <c r="H1711" s="1">
@@ -68901,7 +69146,7 @@
       <c r="A1712" t="s">
         <v>3080</v>
       </c>
-      <c r="B1712" s="2" t="s">
+      <c r="B1712" t="s">
         <v>550</v>
       </c>
       <c r="C1712" t="s">
@@ -68916,7 +69161,7 @@
       <c r="F1712">
         <v>0</v>
       </c>
-      <c r="G1712" s="2">
+      <c r="G1712">
         <v>0</v>
       </c>
       <c r="H1712" s="1">
@@ -68936,7 +69181,7 @@
       <c r="A1713" t="s">
         <v>3081</v>
       </c>
-      <c r="B1713" s="2" t="s">
+      <c r="B1713" t="s">
         <v>550</v>
       </c>
       <c r="C1713" t="s">
@@ -68951,7 +69196,7 @@
       <c r="F1713">
         <v>1</v>
       </c>
-      <c r="G1713" s="2">
+      <c r="G1713">
         <v>3.2</v>
       </c>
       <c r="H1713" s="1">
@@ -68971,7 +69216,7 @@
       <c r="A1714" t="s">
         <v>3082</v>
       </c>
-      <c r="B1714" s="2" t="s">
+      <c r="B1714" t="s">
         <v>550</v>
       </c>
       <c r="C1714" t="s">
@@ -68986,7 +69231,7 @@
       <c r="F1714">
         <v>1</v>
       </c>
-      <c r="G1714" s="2">
+      <c r="G1714">
         <v>3.2</v>
       </c>
       <c r="H1714" s="1">
@@ -69006,7 +69251,7 @@
       <c r="A1715" t="s">
         <v>3083</v>
       </c>
-      <c r="B1715" s="2" t="s">
+      <c r="B1715" t="s">
         <v>550</v>
       </c>
       <c r="C1715" t="s">
@@ -69021,7 +69266,7 @@
       <c r="F1715">
         <v>1</v>
       </c>
-      <c r="G1715" s="2">
+      <c r="G1715">
         <v>4.7</v>
       </c>
       <c r="H1715" s="1">
@@ -69041,7 +69286,7 @@
       <c r="A1716" t="s">
         <v>3084</v>
       </c>
-      <c r="B1716" s="2" t="s">
+      <c r="B1716" t="s">
         <v>550</v>
       </c>
       <c r="C1716" t="s">
@@ -69056,7 +69301,7 @@
       <c r="F1716">
         <v>1</v>
       </c>
-      <c r="G1716" s="2">
+      <c r="G1716">
         <v>1.1000000000000001</v>
       </c>
       <c r="H1716" s="1">
@@ -69076,7 +69321,7 @@
       <c r="A1717" t="s">
         <v>3085</v>
       </c>
-      <c r="B1717" s="2" t="s">
+      <c r="B1717" t="s">
         <v>550</v>
       </c>
       <c r="C1717" t="s">
@@ -69091,7 +69336,7 @@
       <c r="F1717">
         <v>1</v>
       </c>
-      <c r="G1717" s="2">
+      <c r="G1717">
         <v>1.5</v>
       </c>
       <c r="H1717" s="1">
@@ -69105,6 +69350,1365 @@
       </c>
       <c r="K1717">
         <v>36</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1718" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B1718" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D1718" t="s">
+        <v>3087</v>
+      </c>
+      <c r="E1718">
+        <v>1</v>
+      </c>
+      <c r="F1718">
+        <v>1</v>
+      </c>
+      <c r="G1718" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1718" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1718" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1718" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1718">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1719" t="s">
+        <v>3088</v>
+      </c>
+      <c r="B1719" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>3089</v>
+      </c>
+      <c r="D1719" t="s">
+        <v>3090</v>
+      </c>
+      <c r="E1719">
+        <v>2</v>
+      </c>
+      <c r="F1719">
+        <v>1</v>
+      </c>
+      <c r="G1719" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1719" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1719" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1719" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1719">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1720" t="s">
+        <v>3091</v>
+      </c>
+      <c r="B1720" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>3089</v>
+      </c>
+      <c r="D1720" t="s">
+        <v>813</v>
+      </c>
+      <c r="E1720">
+        <v>1</v>
+      </c>
+      <c r="F1720">
+        <v>1</v>
+      </c>
+      <c r="G1720" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1720" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1720" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1720" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1720">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1721" t="s">
+        <v>3092</v>
+      </c>
+      <c r="B1721" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>3093</v>
+      </c>
+      <c r="D1721" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E1721">
+        <v>2.5</v>
+      </c>
+      <c r="F1721">
+        <v>1</v>
+      </c>
+      <c r="G1721" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H1721" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1721" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1721" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1721">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1722" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B1722" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>3095</v>
+      </c>
+      <c r="D1722" t="s">
+        <v>2962</v>
+      </c>
+      <c r="E1722">
+        <v>1</v>
+      </c>
+      <c r="F1722">
+        <v>1</v>
+      </c>
+      <c r="G1722" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1722" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1722" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1722" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1722">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1723" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B1723" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>3097</v>
+      </c>
+      <c r="D1723" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1723">
+        <v>1.5</v>
+      </c>
+      <c r="F1723">
+        <v>1</v>
+      </c>
+      <c r="G1723" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H1723" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1723" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1723" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1723">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1724" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B1724" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D1724" t="s">
+        <v>2535</v>
+      </c>
+      <c r="E1724">
+        <v>1</v>
+      </c>
+      <c r="F1724">
+        <v>1</v>
+      </c>
+      <c r="G1724" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1724" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1724" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1724" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1724">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1725" t="s">
+        <v>3099</v>
+      </c>
+      <c r="B1725" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D1725" t="s">
+        <v>3100</v>
+      </c>
+      <c r="E1725">
+        <v>1</v>
+      </c>
+      <c r="F1725">
+        <v>1</v>
+      </c>
+      <c r="G1725" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1725" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1725" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1725" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1725">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1726" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B1726" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>3102</v>
+      </c>
+      <c r="D1726" t="s">
+        <v>3103</v>
+      </c>
+      <c r="E1726">
+        <v>2</v>
+      </c>
+      <c r="F1726">
+        <v>1</v>
+      </c>
+      <c r="G1726" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1726" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1726" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1726" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1726">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1727" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B1727" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>3105</v>
+      </c>
+      <c r="D1727" t="s">
+        <v>3106</v>
+      </c>
+      <c r="E1727">
+        <v>1</v>
+      </c>
+      <c r="F1727">
+        <v>1</v>
+      </c>
+      <c r="G1727" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1727" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1727" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1727" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1727">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1728" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B1728" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>3108</v>
+      </c>
+      <c r="D1728" t="s">
+        <v>2533</v>
+      </c>
+      <c r="E1728">
+        <v>1</v>
+      </c>
+      <c r="F1728">
+        <v>1</v>
+      </c>
+      <c r="G1728" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1728" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1728" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1728" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1728">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1729" t="s">
+        <v>3109</v>
+      </c>
+      <c r="B1729" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D1729" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1729">
+        <v>1.5</v>
+      </c>
+      <c r="F1729">
+        <v>1</v>
+      </c>
+      <c r="G1729" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H1729" s="1">
+        <v>45544</v>
+      </c>
+      <c r="I1729" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1729" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1729">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1730" t="s">
+        <v>3110</v>
+      </c>
+      <c r="B1730" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>3111</v>
+      </c>
+      <c r="D1730" t="s">
+        <v>3112</v>
+      </c>
+      <c r="E1730">
+        <v>4.5</v>
+      </c>
+      <c r="F1730">
+        <v>1</v>
+      </c>
+      <c r="G1730" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="H1730" s="1">
+        <v>45545</v>
+      </c>
+      <c r="I1730" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1730" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1730">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1731" t="s">
+        <v>3113</v>
+      </c>
+      <c r="B1731" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>3114</v>
+      </c>
+      <c r="D1731" t="s">
+        <v>3115</v>
+      </c>
+      <c r="E1731">
+        <v>3.1</v>
+      </c>
+      <c r="F1731">
+        <v>1</v>
+      </c>
+      <c r="G1731" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="H1731" s="1">
+        <v>45545</v>
+      </c>
+      <c r="I1731" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1731" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1731">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1732" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B1732" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>3117</v>
+      </c>
+      <c r="D1732" t="s">
+        <v>848</v>
+      </c>
+      <c r="E1732">
+        <v>8</v>
+      </c>
+      <c r="F1732">
+        <v>1</v>
+      </c>
+      <c r="G1732" s="2">
+        <v>8</v>
+      </c>
+      <c r="H1732" s="1">
+        <v>45545</v>
+      </c>
+      <c r="I1732" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1732" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1732">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1733" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B1733" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>3117</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>3119</v>
+      </c>
+      <c r="E1733">
+        <v>3</v>
+      </c>
+      <c r="F1733">
+        <v>1</v>
+      </c>
+      <c r="G1733" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1733" s="1">
+        <v>45545</v>
+      </c>
+      <c r="I1733" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1733" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1733">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1734" t="s">
+        <v>3120</v>
+      </c>
+      <c r="B1734" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>3121</v>
+      </c>
+      <c r="D1734" t="s">
+        <v>3122</v>
+      </c>
+      <c r="E1734">
+        <v>3.6</v>
+      </c>
+      <c r="F1734">
+        <v>1</v>
+      </c>
+      <c r="G1734" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="H1734" s="1">
+        <v>45545</v>
+      </c>
+      <c r="I1734" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1734" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1734">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1735" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B1735" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>3121</v>
+      </c>
+      <c r="D1735" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E1735">
+        <v>1.5</v>
+      </c>
+      <c r="F1735">
+        <v>1</v>
+      </c>
+      <c r="G1735" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H1735" s="1">
+        <v>45545</v>
+      </c>
+      <c r="I1735" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1735" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1735">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1736" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B1736" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>3125</v>
+      </c>
+      <c r="D1736" t="s">
+        <v>848</v>
+      </c>
+      <c r="E1736">
+        <v>12.7</v>
+      </c>
+      <c r="F1736">
+        <v>0</v>
+      </c>
+      <c r="G1736" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1736" s="1">
+        <v>45546</v>
+      </c>
+      <c r="I1736" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1736" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1736">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1737" t="s">
+        <v>3126</v>
+      </c>
+      <c r="B1737" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>3127</v>
+      </c>
+      <c r="D1737" t="s">
+        <v>3128</v>
+      </c>
+      <c r="E1737">
+        <v>2.5</v>
+      </c>
+      <c r="F1737">
+        <v>0</v>
+      </c>
+      <c r="G1737" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1737" s="1">
+        <v>45546</v>
+      </c>
+      <c r="I1737" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1737" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1737">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1738" t="s">
+        <v>3129</v>
+      </c>
+      <c r="B1738" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>3130</v>
+      </c>
+      <c r="D1738" t="s">
+        <v>1946</v>
+      </c>
+      <c r="E1738">
+        <v>2.5</v>
+      </c>
+      <c r="F1738">
+        <v>1</v>
+      </c>
+      <c r="G1738" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H1738" s="1">
+        <v>45546</v>
+      </c>
+      <c r="I1738" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1738" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1738">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1739" t="s">
+        <v>3131</v>
+      </c>
+      <c r="B1739" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>3130</v>
+      </c>
+      <c r="D1739" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E1739">
+        <v>2.5</v>
+      </c>
+      <c r="F1739">
+        <v>0</v>
+      </c>
+      <c r="G1739" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1739" s="1">
+        <v>45546</v>
+      </c>
+      <c r="I1739" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1739" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1739">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1740" t="s">
+        <v>3132</v>
+      </c>
+      <c r="B1740" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>3130</v>
+      </c>
+      <c r="D1740" t="s">
+        <v>3133</v>
+      </c>
+      <c r="E1740">
+        <v>1.3</v>
+      </c>
+      <c r="F1740">
+        <v>1</v>
+      </c>
+      <c r="G1740" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="H1740" s="1">
+        <v>45546</v>
+      </c>
+      <c r="I1740" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1740" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1740">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1741" t="s">
+        <v>3134</v>
+      </c>
+      <c r="B1741" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>3130</v>
+      </c>
+      <c r="D1741" t="s">
+        <v>3135</v>
+      </c>
+      <c r="E1741">
+        <v>0.5</v>
+      </c>
+      <c r="F1741">
+        <v>1</v>
+      </c>
+      <c r="G1741" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H1741" s="1">
+        <v>45546</v>
+      </c>
+      <c r="I1741" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1741" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1741">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1742" t="s">
+        <v>3136</v>
+      </c>
+      <c r="B1742" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>3137</v>
+      </c>
+      <c r="D1742" t="s">
+        <v>848</v>
+      </c>
+      <c r="E1742">
+        <v>4.2</v>
+      </c>
+      <c r="F1742">
+        <v>0</v>
+      </c>
+      <c r="G1742" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1742" s="1">
+        <v>45547</v>
+      </c>
+      <c r="I1742" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1742" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1742">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1743" t="s">
+        <v>3138</v>
+      </c>
+      <c r="B1743" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>3139</v>
+      </c>
+      <c r="D1743" t="s">
+        <v>3140</v>
+      </c>
+      <c r="E1743">
+        <v>2</v>
+      </c>
+      <c r="F1743">
+        <v>0</v>
+      </c>
+      <c r="G1743" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1743" s="1">
+        <v>45547</v>
+      </c>
+      <c r="I1743" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1743" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1743">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1744" t="s">
+        <v>3141</v>
+      </c>
+      <c r="B1744" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>3142</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>3143</v>
+      </c>
+      <c r="E1744">
+        <v>5.4</v>
+      </c>
+      <c r="F1744">
+        <v>1</v>
+      </c>
+      <c r="G1744" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="H1744" s="1">
+        <v>45547</v>
+      </c>
+      <c r="I1744" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1744" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1744">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1745" t="s">
+        <v>3144</v>
+      </c>
+      <c r="B1745" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>3142</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>3145</v>
+      </c>
+      <c r="E1745">
+        <v>0.9</v>
+      </c>
+      <c r="F1745">
+        <v>1</v>
+      </c>
+      <c r="G1745" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="H1745" s="1">
+        <v>45547</v>
+      </c>
+      <c r="I1745" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1745" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1745">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1746" t="s">
+        <v>3146</v>
+      </c>
+      <c r="B1746" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1746" t="s">
+        <v>3147</v>
+      </c>
+      <c r="D1746" t="s">
+        <v>3148</v>
+      </c>
+      <c r="E1746">
+        <v>4.7</v>
+      </c>
+      <c r="F1746">
+        <v>0</v>
+      </c>
+      <c r="G1746" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1746" s="1">
+        <v>45547</v>
+      </c>
+      <c r="I1746" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1746" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1746">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1747" t="s">
+        <v>3149</v>
+      </c>
+      <c r="B1747" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1747" t="s">
+        <v>3150</v>
+      </c>
+      <c r="D1747" t="s">
+        <v>3151</v>
+      </c>
+      <c r="E1747">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F1747">
+        <v>1</v>
+      </c>
+      <c r="G1747" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H1747" s="1">
+        <v>45548</v>
+      </c>
+      <c r="I1747" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1747" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1747">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1748" t="s">
+        <v>3152</v>
+      </c>
+      <c r="B1748" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>3150</v>
+      </c>
+      <c r="D1748" t="s">
+        <v>3153</v>
+      </c>
+      <c r="E1748">
+        <v>7.9</v>
+      </c>
+      <c r="F1748">
+        <v>1</v>
+      </c>
+      <c r="G1748" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="H1748" s="1">
+        <v>45548</v>
+      </c>
+      <c r="I1748" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1748" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1748">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1749" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B1749" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1749" t="s">
+        <v>3150</v>
+      </c>
+      <c r="D1749" t="s">
+        <v>3155</v>
+      </c>
+      <c r="E1749">
+        <v>3</v>
+      </c>
+      <c r="F1749">
+        <v>1</v>
+      </c>
+      <c r="G1749" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1749" s="1">
+        <v>45548</v>
+      </c>
+      <c r="I1749" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1749" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1749">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1750" t="s">
+        <v>3156</v>
+      </c>
+      <c r="B1750" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1750" t="s">
+        <v>3157</v>
+      </c>
+      <c r="D1750" t="s">
+        <v>3158</v>
+      </c>
+      <c r="F1750">
+        <v>0</v>
+      </c>
+      <c r="G1750" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1750" s="1">
+        <v>45548</v>
+      </c>
+      <c r="I1750" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1750" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1750">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1751" t="s">
+        <v>3159</v>
+      </c>
+      <c r="B1751" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1751" t="s">
+        <v>3157</v>
+      </c>
+      <c r="D1751" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F1751">
+        <v>1</v>
+      </c>
+      <c r="G1751" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1751" s="1">
+        <v>45548</v>
+      </c>
+      <c r="I1751" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1751" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1751">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1752" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B1752" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1752" t="s">
+        <v>3161</v>
+      </c>
+      <c r="D1752" t="s">
+        <v>3140</v>
+      </c>
+      <c r="E1752">
+        <v>2</v>
+      </c>
+      <c r="F1752">
+        <v>0</v>
+      </c>
+      <c r="G1752" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1752" s="1">
+        <v>45549</v>
+      </c>
+      <c r="I1752" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1752" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1752">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1753" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B1753" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1753" t="s">
+        <v>3161</v>
+      </c>
+      <c r="D1753" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E1753">
+        <v>2</v>
+      </c>
+      <c r="F1753">
+        <v>1</v>
+      </c>
+      <c r="G1753" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1753" s="1">
+        <v>45549</v>
+      </c>
+      <c r="I1753" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1753" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1753">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1754" t="s">
+        <v>3163</v>
+      </c>
+      <c r="B1754" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1754" t="s">
+        <v>3164</v>
+      </c>
+      <c r="D1754" t="s">
+        <v>3140</v>
+      </c>
+      <c r="E1754">
+        <v>1.5</v>
+      </c>
+      <c r="F1754">
+        <v>0</v>
+      </c>
+      <c r="G1754" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1754" s="1">
+        <v>45549</v>
+      </c>
+      <c r="I1754" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1754" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1754">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1755" t="s">
+        <v>3165</v>
+      </c>
+      <c r="B1755" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1755" t="s">
+        <v>3164</v>
+      </c>
+      <c r="D1755" t="s">
+        <v>3143</v>
+      </c>
+      <c r="E1755">
+        <v>5.4</v>
+      </c>
+      <c r="F1755">
+        <v>1</v>
+      </c>
+      <c r="G1755" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="H1755" s="1">
+        <v>45549</v>
+      </c>
+      <c r="I1755" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1755" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1755">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1756" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B1756" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C1756" t="s">
+        <v>3167</v>
+      </c>
+      <c r="D1756" t="s">
+        <v>3168</v>
+      </c>
+      <c r="E1756">
+        <v>0.9</v>
+      </c>
+      <c r="F1756">
+        <v>0</v>
+      </c>
+      <c r="G1756" s="2">
+        <v>0</v>
+      </c>
+      <c r="H1756" s="1">
+        <v>45549</v>
+      </c>
+      <c r="I1756" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1756" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1756">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>